<commit_message>
Completed testing, still need to fix some bugs and finalize the formatting and complete all TODOs
</commit_message>
<xml_diff>
--- a/app/Export/OverallAnalysisCurrent.xlsx
+++ b/app/Export/OverallAnalysisCurrent.xlsx
@@ -3132,7 +3132,7 @@
         <v>12</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -3619,7 +3619,7 @@
         <v>2</v>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K33" t="n">
         <v>0</v>
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="W33" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="X33" t="n">
         <v>0</v>
@@ -3673,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="AB33" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34">
@@ -4504,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" t="n">
         <v>0</v>
@@ -8825,7 +8825,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O86" t="n">
         <v>0</v>
@@ -8861,7 +8861,7 @@
         <v>2</v>
       </c>
       <c r="Z86" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AA86" t="n">
         <v>0</v>
@@ -10969,10 +10969,10 @@
         <v>0</v>
       </c>
       <c r="J108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K108" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L108" t="n">
         <v>6</v>
@@ -14438,7 +14438,7 @@
         <v>0</v>
       </c>
       <c r="W143" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X143" t="n">
         <v>1</v>
@@ -15480,7 +15480,7 @@
         <v>0</v>
       </c>
       <c r="K154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L154" t="n">
         <v>0</v>
@@ -35116,7 +35116,7 @@
         <v>0</v>
       </c>
       <c r="W354" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X354" t="n">
         <v>0</v>
@@ -64575,7 +64575,7 @@
         <v>0</v>
       </c>
       <c r="J655" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K655" t="n">
         <v>0</v>
@@ -67417,10 +67417,10 @@
         <v>0</v>
       </c>
       <c r="J684" t="n">
+        <v>2</v>
+      </c>
+      <c r="K684" t="n">
         <v>1</v>
-      </c>
-      <c r="K684" t="n">
-        <v>0</v>
       </c>
       <c r="L684" t="n">
         <v>0</v>
@@ -74880,7 +74880,7 @@
         <v>10</v>
       </c>
       <c r="O760" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P760" t="n">
         <v>0</v>
@@ -74892,13 +74892,13 @@
         <v>0</v>
       </c>
       <c r="S760" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T760" t="n">
         <v>0</v>
       </c>
       <c r="U760" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="V760" t="n">
         <v>0</v>

</xml_diff>